<commit_message>
updated all test packs to have a valid Nominated Pharmacy Type column
</commit_message>
<xml_diff>
--- a/tool/e2e-tests/test-packs/Post Dated Prescriptions Test Pack.xlsx
+++ b/tool/e2e-tests/test-packs/Post Dated Prescriptions Test Pack.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\clients\NHS\electronic-prescription-service-api\tool\e2e-tests\test-packs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathew.arnold\electronic-prescription-service-api\tool\e2e-tests\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B79DFF-D37A-48E8-BB01-C1657CBB0DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643F5EB7-8F85-4FF7-97B2-002D01FCCBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{DE2866F1-D839-4AD2-B338-FF4A1D84F7C7}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="16186" xr2:uid="{DE2866F1-D839-4AD2-B338-FF4A1D84F7C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Prescriptions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Prescriptions!$A$1:$V$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Prescriptions!$A$1:$W$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Quantity</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>3000-12-31</t>
+  </si>
+  <si>
+    <t>Nominated Pharmacy Type</t>
+  </si>
+  <si>
+    <t>P1</t>
   </si>
 </sst>
 </file>
@@ -529,36 +535,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90350D13-E130-47A5-A64D-77E01FA3003F}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="121.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1328125" customWidth="1"/>
-    <col min="14" max="14" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="19.1328125" customWidth="1"/>
-    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="58.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="55.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.19921875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="121.1484375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.84765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1484375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.1484375" customWidth="1"/>
+    <col min="15" max="15" width="19.1484375" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="19.1484375" customWidth="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="58.546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="55.546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -572,61 +578,64 @@
         <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -640,39 +649,42 @@
         <v>18</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>28</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>99999999</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>11111111</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="3" t="s">
+      <c r="O2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -686,37 +698,40 @@
         <v>18</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>28</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>99999999</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>35</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>11111111</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="T3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="U3" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V3" xr:uid="{90350D13-E130-47A5-A64D-77E01FA3003F}"/>
+  <autoFilter ref="A1:W3" xr:uid="{90350D13-E130-47A5-A64D-77E01FA3003F}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>